<commit_message>
Switched GDP from constant to current prices
This was done to ensure that all price-related data (sales prices, disposable income and national GDP) is measured in current prices, making them both directly comparable to each other and keeping the numbers the same as they appear in the source.
</commit_message>
<xml_diff>
--- a/Input data/WEO_Data_Denmark.xlsx
+++ b/Input data/WEO_Data_Denmark.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/Documents/Hsng prices/Input data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00912291-36BC-4E18-8747-4E5B0199266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{00912291-36BC-4E18-8747-4E5B0199266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8514875-5182-4494-9144-54D47E3951F7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WEO_Data_Denmark" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>WEO Country Code</t>
-  </si>
-  <si>
-    <t>WEO Subject Code</t>
   </si>
   <si>
     <t>Country</t>
@@ -40,19 +37,10 @@
     <t>Scale</t>
   </si>
   <si>
-    <t>Country/Series-specific Notes</t>
-  </si>
-  <si>
     <t>Estimates Start After</t>
   </si>
   <si>
-    <t>NGDP_R</t>
-  </si>
-  <si>
     <t>Denmark</t>
-  </si>
-  <si>
-    <t>Gross domestic product, constant prices</t>
   </si>
   <si>
     <t>National currency</t>
@@ -61,19 +49,7 @@
     <t>Billions</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 National accounts manual used: European System of Accounts (ESA) 2010 GDP valuation: Market prices Reporting in calendar year: Yes Start/end months of reporting year: January/December Base year: 2010 Chain-weighted: Yes, from 1980 Primary domestic currency: Danish krone Data last updated: 09/2023</t>
-  </si>
-  <si>
-    <t>NGDP_RPCH</t>
-  </si>
-  <si>
     <t>Percent change</t>
-  </si>
-  <si>
-    <t>See notes for:  Gross domestic product, constant prices (National currency).</t>
-  </si>
-  <si>
-    <t>PCPI</t>
   </si>
   <si>
     <t>Inflation, average consumer prices</t>
@@ -82,28 +58,7 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 Harmonized prices: Yes Base year: 2015 Primary domestic currency: Danish krone Data last updated: 09/2023</t>
-  </si>
-  <si>
-    <t>PCPIPCH</t>
-  </si>
-  <si>
-    <t>See notes for:  Inflation, average consumer prices (Index).</t>
-  </si>
-  <si>
-    <t>PCPIE</t>
-  </si>
-  <si>
     <t>Inflation, end of period consumer prices</t>
-  </si>
-  <si>
-    <t>PCPIEPCH</t>
-  </si>
-  <si>
-    <t>See notes for:  Inflation, end of period consumer prices (Index).</t>
-  </si>
-  <si>
-    <t>LP</t>
   </si>
   <si>
     <t>Population</t>
@@ -115,16 +70,16 @@
     <t>Millions</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 Primary domestic currency: Danish krone Data last updated: 09/2023</t>
+    <t>International Monetary Fund, World Economic Outlook Database, October 2023</t>
   </si>
   <si>
-    <t>International Monetary Fund, World Economic Outlook Database, October 2023</t>
+    <t>Gross domestic product, current prices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -979,14 +934,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,1362 +959,1150 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1">
+        <v>1980</v>
+      </c>
+      <c r="G1">
+        <v>1981</v>
+      </c>
+      <c r="H1">
+        <v>1982</v>
+      </c>
+      <c r="I1">
+        <v>1983</v>
+      </c>
+      <c r="J1">
+        <v>1984</v>
+      </c>
+      <c r="K1">
+        <v>1985</v>
+      </c>
+      <c r="L1">
+        <v>1986</v>
+      </c>
+      <c r="M1">
+        <v>1987</v>
+      </c>
+      <c r="N1">
+        <v>1988</v>
+      </c>
+      <c r="O1">
+        <v>1989</v>
+      </c>
+      <c r="P1">
+        <v>1990</v>
+      </c>
+      <c r="Q1">
+        <v>1991</v>
+      </c>
+      <c r="R1">
+        <v>1992</v>
+      </c>
+      <c r="S1">
+        <v>1993</v>
+      </c>
+      <c r="T1">
+        <v>1994</v>
+      </c>
+      <c r="U1">
+        <v>1995</v>
+      </c>
+      <c r="V1">
+        <v>1996</v>
+      </c>
+      <c r="W1">
+        <v>1997</v>
+      </c>
+      <c r="X1">
+        <v>1998</v>
+      </c>
+      <c r="Y1">
+        <v>1999</v>
+      </c>
+      <c r="Z1">
+        <v>2000</v>
+      </c>
+      <c r="AA1">
+        <v>2001</v>
+      </c>
+      <c r="AB1">
+        <v>2002</v>
+      </c>
+      <c r="AC1">
+        <v>2003</v>
+      </c>
+      <c r="AD1">
+        <v>2004</v>
+      </c>
+      <c r="AE1">
+        <v>2005</v>
+      </c>
+      <c r="AF1">
+        <v>2006</v>
+      </c>
+      <c r="AG1">
+        <v>2007</v>
+      </c>
+      <c r="AH1">
+        <v>2008</v>
+      </c>
+      <c r="AI1">
+        <v>2009</v>
+      </c>
+      <c r="AJ1">
+        <v>2010</v>
+      </c>
+      <c r="AK1">
+        <v>2011</v>
+      </c>
+      <c r="AL1">
+        <v>2012</v>
+      </c>
+      <c r="AM1">
+        <v>2013</v>
+      </c>
+      <c r="AN1">
+        <v>2014</v>
+      </c>
+      <c r="AO1">
+        <v>2015</v>
+      </c>
+      <c r="AP1">
+        <v>2016</v>
+      </c>
+      <c r="AQ1">
+        <v>2017</v>
+      </c>
+      <c r="AR1">
+        <v>2018</v>
+      </c>
+      <c r="AS1">
+        <v>2019</v>
+      </c>
+      <c r="AT1">
+        <v>2020</v>
+      </c>
+      <c r="AU1">
+        <v>2021</v>
+      </c>
+      <c r="AV1">
+        <v>2022</v>
+      </c>
+      <c r="AW1">
+        <v>2023</v>
+      </c>
+      <c r="AX1">
+        <v>2024</v>
+      </c>
+      <c r="AY1">
+        <v>2025</v>
+      </c>
+      <c r="AZ1">
+        <v>2026</v>
+      </c>
+      <c r="BA1">
+        <v>2027</v>
+      </c>
+      <c r="BB1">
+        <v>2028</v>
+      </c>
+      <c r="BC1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>1980</v>
-      </c>
-      <c r="I1">
-        <v>1981</v>
-      </c>
-      <c r="J1">
-        <v>1982</v>
-      </c>
-      <c r="K1">
-        <v>1983</v>
-      </c>
-      <c r="L1">
-        <v>1984</v>
-      </c>
-      <c r="M1">
-        <v>1985</v>
-      </c>
-      <c r="N1">
-        <v>1986</v>
-      </c>
-      <c r="O1">
-        <v>1987</v>
-      </c>
-      <c r="P1">
-        <v>1988</v>
-      </c>
-      <c r="Q1">
-        <v>1989</v>
-      </c>
-      <c r="R1">
-        <v>1990</v>
-      </c>
-      <c r="S1">
-        <v>1991</v>
-      </c>
-      <c r="T1">
-        <v>1992</v>
-      </c>
-      <c r="U1">
-        <v>1993</v>
-      </c>
-      <c r="V1">
-        <v>1994</v>
-      </c>
-      <c r="W1">
-        <v>1995</v>
-      </c>
-      <c r="X1">
-        <v>1996</v>
-      </c>
-      <c r="Y1">
-        <v>1997</v>
-      </c>
-      <c r="Z1">
-        <v>1998</v>
-      </c>
-      <c r="AA1">
-        <v>1999</v>
-      </c>
-      <c r="AB1">
-        <v>2000</v>
-      </c>
-      <c r="AC1">
-        <v>2001</v>
-      </c>
-      <c r="AD1">
-        <v>2002</v>
-      </c>
-      <c r="AE1">
-        <v>2003</v>
-      </c>
-      <c r="AF1">
-        <v>2004</v>
-      </c>
-      <c r="AG1">
-        <v>2005</v>
-      </c>
-      <c r="AH1">
-        <v>2006</v>
-      </c>
-      <c r="AI1">
-        <v>2007</v>
-      </c>
-      <c r="AJ1">
-        <v>2008</v>
-      </c>
-      <c r="AK1">
-        <v>2009</v>
-      </c>
-      <c r="AL1">
-        <v>2010</v>
-      </c>
-      <c r="AM1">
-        <v>2011</v>
-      </c>
-      <c r="AN1">
-        <v>2012</v>
-      </c>
-      <c r="AO1">
-        <v>2013</v>
-      </c>
-      <c r="AP1">
-        <v>2014</v>
-      </c>
-      <c r="AQ1">
-        <v>2015</v>
-      </c>
-      <c r="AR1">
-        <v>2016</v>
-      </c>
-      <c r="AS1">
-        <v>2017</v>
-      </c>
-      <c r="AT1">
-        <v>2018</v>
-      </c>
-      <c r="AU1">
-        <v>2019</v>
-      </c>
-      <c r="AV1">
-        <v>2020</v>
-      </c>
-      <c r="AW1">
-        <v>2021</v>
-      </c>
-      <c r="AX1">
-        <v>2022</v>
-      </c>
-      <c r="AY1">
-        <v>2023</v>
-      </c>
-      <c r="AZ1">
-        <v>2024</v>
-      </c>
-      <c r="BA1">
-        <v>2025</v>
-      </c>
-      <c r="BB1">
-        <v>2026</v>
-      </c>
-      <c r="BC1">
-        <v>2027</v>
-      </c>
-      <c r="BD1">
-        <v>2028</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>128</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1048.0999999999999</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1041.2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1079.5</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1107.5</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1153.7</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1199.9000000000001</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1258.7</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1261.9000000000001</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1261.8</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1269.9000000000001</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1288.5999999999999</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1306.5999999999999</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1332.2</v>
+      <c r="F2">
+        <v>400.86700000000002</v>
+      </c>
+      <c r="G2">
+        <v>440.78100000000001</v>
+      </c>
+      <c r="H2">
+        <v>503.38400000000001</v>
+      </c>
+      <c r="I2">
+        <v>554.59699999999998</v>
+      </c>
+      <c r="J2">
+        <v>612.12900000000002</v>
+      </c>
+      <c r="K2">
+        <v>663.95399999999995</v>
+      </c>
+      <c r="L2">
+        <v>712.64499999999998</v>
+      </c>
+      <c r="M2">
+        <v>748.42700000000002</v>
+      </c>
+      <c r="N2">
+        <v>777.84400000000005</v>
+      </c>
+      <c r="O2">
+        <v>821.73400000000004</v>
+      </c>
+      <c r="P2">
+        <v>855.55700000000002</v>
+      </c>
+      <c r="Q2">
+        <v>890.55100000000004</v>
+      </c>
+      <c r="R2">
+        <v>923.01499999999999</v>
+      </c>
+      <c r="S2">
+        <v>928.46600000000001</v>
+      </c>
+      <c r="T2">
+        <v>993.28700000000003</v>
       </c>
       <c r="U2" s="1">
-        <v>1332.3</v>
+        <v>1036.4829999999999</v>
       </c>
       <c r="V2" s="1">
-        <v>1403.3</v>
+        <v>1088.0239999999999</v>
       </c>
       <c r="W2" s="1">
-        <v>1445.8</v>
+        <v>1146.1289999999999</v>
       </c>
       <c r="X2" s="1">
-        <v>1487.8</v>
+        <v>1185.9870000000001</v>
       </c>
       <c r="Y2" s="1">
-        <v>1536.3</v>
+        <v>1241.521</v>
       </c>
       <c r="Z2" s="1">
-        <v>1570.3</v>
+        <v>1326.9110000000001</v>
       </c>
       <c r="AA2" s="1">
-        <v>1616.6</v>
+        <v>1371.5260000000001</v>
       </c>
       <c r="AB2" s="1">
-        <v>1677.2</v>
+        <v>1410.2719999999999</v>
       </c>
       <c r="AC2" s="1">
-        <v>1691</v>
+        <v>1436.751</v>
       </c>
       <c r="AD2" s="1">
-        <v>1698.9</v>
+        <v>1506.002</v>
       </c>
       <c r="AE2" s="1">
-        <v>1705.5</v>
+        <v>1585.9829999999999</v>
       </c>
       <c r="AF2" s="1">
-        <v>1751</v>
+        <v>1682.26</v>
       </c>
       <c r="AG2" s="1">
-        <v>1792</v>
+        <v>1738.846</v>
       </c>
       <c r="AH2" s="1">
-        <v>1862.1</v>
+        <v>1801.47</v>
       </c>
       <c r="AI2" s="1">
-        <v>1879</v>
+        <v>1722.143</v>
       </c>
       <c r="AJ2" s="1">
-        <v>1869.4</v>
+        <v>1810.9259999999999</v>
       </c>
       <c r="AK2" s="1">
-        <v>1777.7</v>
+        <v>1846.854</v>
       </c>
       <c r="AL2" s="1">
-        <v>1810.9</v>
+        <v>1895.002</v>
       </c>
       <c r="AM2" s="1">
-        <v>1835.1</v>
+        <v>1929.6769999999999</v>
       </c>
       <c r="AN2" s="1">
-        <v>1839.3</v>
+        <v>1981.165</v>
       </c>
       <c r="AO2" s="1">
-        <v>1856.5</v>
+        <v>2036.356</v>
       </c>
       <c r="AP2" s="1">
-        <v>1886.5</v>
+        <v>2107.8090000000002</v>
       </c>
       <c r="AQ2" s="1">
-        <v>1930.7</v>
+        <v>2192.96</v>
       </c>
       <c r="AR2" s="1">
-        <v>1993.4</v>
+        <v>2253.3150000000001</v>
       </c>
       <c r="AS2" s="1">
-        <v>2049.6</v>
+        <v>2310.9549999999999</v>
       </c>
       <c r="AT2" s="1">
-        <v>2090.4</v>
+        <v>2320.9119999999998</v>
       </c>
       <c r="AU2" s="1">
-        <v>2121.6</v>
+        <v>2550.605</v>
       </c>
       <c r="AV2" s="1">
-        <v>2070.1999999999998</v>
+        <v>2838.4189999999999</v>
       </c>
       <c r="AW2" s="1">
-        <v>2211.9</v>
+        <v>2882.625</v>
       </c>
       <c r="AX2" s="1">
-        <v>2272.3000000000002</v>
+        <v>2968.6860000000001</v>
       </c>
       <c r="AY2" s="1">
-        <v>2310.9290000000001</v>
+        <v>3070.6149999999998</v>
       </c>
       <c r="AZ2" s="1">
-        <v>2343.2820000000002</v>
+        <v>3177.7919999999999</v>
       </c>
       <c r="BA2" s="1">
-        <v>2371.4009999999998</v>
+        <v>3287.8820000000001</v>
       </c>
       <c r="BB2" s="1">
-        <v>2402.23</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>2433.4589999999998</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>2465.0940000000001</v>
-      </c>
-      <c r="BE2">
+        <v>3403.3580000000002</v>
+      </c>
+      <c r="BC2">
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>36.194000000000003</v>
+      </c>
+      <c r="G3">
+        <v>40.435000000000002</v>
       </c>
       <c r="H3">
-        <v>-0.48399999999999999</v>
+        <v>44.536999999999999</v>
       </c>
       <c r="I3">
-        <v>-0.65800000000000003</v>
+        <v>47.582000000000001</v>
       </c>
       <c r="J3">
-        <v>3.6779999999999999</v>
+        <v>50.6</v>
       </c>
       <c r="K3">
-        <v>2.5939999999999999</v>
+        <v>52.959000000000003</v>
       </c>
       <c r="L3">
-        <v>4.1719999999999997</v>
+        <v>54.927999999999997</v>
       </c>
       <c r="M3">
-        <v>4.0049999999999999</v>
+        <v>57.113999999999997</v>
       </c>
       <c r="N3">
-        <v>4.9000000000000004</v>
+        <v>59.698</v>
       </c>
       <c r="O3">
-        <v>0.254</v>
+        <v>62.552</v>
       </c>
       <c r="P3">
-        <v>-8.0000000000000002E-3</v>
+        <v>64.207999999999998</v>
       </c>
       <c r="Q3">
-        <v>0.64200000000000002</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="R3">
-        <v>1.4730000000000001</v>
+        <v>66.875</v>
       </c>
       <c r="S3">
-        <v>1.397</v>
+        <v>67.457999999999998</v>
       </c>
       <c r="T3">
-        <v>1.9590000000000001</v>
+        <v>68.7</v>
       </c>
       <c r="U3">
-        <v>8.0000000000000002E-3</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="V3">
-        <v>5.3289999999999997</v>
+        <v>71.566999999999993</v>
       </c>
       <c r="W3">
-        <v>3.0289999999999999</v>
+        <v>72.95</v>
       </c>
       <c r="X3">
-        <v>2.9049999999999998</v>
+        <v>73.908000000000001</v>
       </c>
       <c r="Y3">
-        <v>3.26</v>
+        <v>75.417000000000002</v>
       </c>
       <c r="Z3">
-        <v>2.2130000000000001</v>
+        <v>77.492000000000004</v>
       </c>
       <c r="AA3">
-        <v>2.948</v>
+        <v>79.25</v>
       </c>
       <c r="AB3">
-        <v>3.7490000000000001</v>
+        <v>81.150000000000006</v>
       </c>
       <c r="AC3">
-        <v>0.82299999999999995</v>
+        <v>82.742000000000004</v>
       </c>
       <c r="AD3">
-        <v>0.46700000000000003</v>
+        <v>83.516999999999996</v>
       </c>
       <c r="AE3">
-        <v>0.38800000000000001</v>
+        <v>84.957999999999998</v>
       </c>
       <c r="AF3">
-        <v>2.6680000000000001</v>
+        <v>86.525000000000006</v>
       </c>
       <c r="AG3">
-        <v>2.3420000000000001</v>
+        <v>87.957999999999998</v>
       </c>
       <c r="AH3">
-        <v>3.9119999999999999</v>
+        <v>91.158000000000001</v>
       </c>
       <c r="AI3">
-        <v>0.90800000000000003</v>
+        <v>92.108000000000004</v>
       </c>
       <c r="AJ3">
-        <v>-0.51100000000000001</v>
+        <v>94.132999999999996</v>
       </c>
       <c r="AK3">
-        <v>-4.9050000000000002</v>
+        <v>96.632999999999996</v>
       </c>
       <c r="AL3">
-        <v>1.8680000000000001</v>
+        <v>98.908000000000001</v>
       </c>
       <c r="AM3">
-        <v>1.3360000000000001</v>
+        <v>99.424999999999997</v>
       </c>
       <c r="AN3">
-        <v>0.22900000000000001</v>
+        <v>99.775000000000006</v>
       </c>
       <c r="AO3">
-        <v>0.93500000000000005</v>
+        <v>100</v>
       </c>
       <c r="AP3">
-        <v>1.6160000000000001</v>
+        <v>100.017</v>
       </c>
       <c r="AQ3">
-        <v>2.343</v>
+        <v>101.075</v>
       </c>
       <c r="AR3">
-        <v>3.2480000000000002</v>
+        <v>101.792</v>
       </c>
       <c r="AS3">
-        <v>2.819</v>
+        <v>102.533</v>
       </c>
       <c r="AT3">
-        <v>1.9910000000000001</v>
+        <v>102.875</v>
       </c>
       <c r="AU3">
-        <v>1.4930000000000001</v>
+        <v>104.875</v>
       </c>
       <c r="AV3">
-        <v>-2.423</v>
+        <v>113.825</v>
       </c>
       <c r="AW3">
-        <v>6.8449999999999998</v>
+        <v>118.54900000000001</v>
       </c>
       <c r="AX3">
-        <v>2.7309999999999999</v>
+        <v>121.86799999999999</v>
       </c>
       <c r="AY3">
-        <v>1.7</v>
+        <v>124.42700000000001</v>
       </c>
       <c r="AZ3">
-        <v>1.4</v>
+        <v>127.04</v>
       </c>
       <c r="BA3">
-        <v>1.2</v>
+        <v>129.58099999999999</v>
       </c>
       <c r="BB3">
-        <v>1.3</v>
+        <v>132.173</v>
       </c>
       <c r="BC3">
-        <v>1.3</v>
-      </c>
-      <c r="BD3">
-        <v>1.3</v>
-      </c>
-      <c r="BE3">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+      <c r="F4">
+        <v>11.339</v>
+      </c>
+      <c r="G4">
+        <v>11.718</v>
       </c>
       <c r="H4">
-        <v>36.194000000000003</v>
+        <v>10.146000000000001</v>
       </c>
       <c r="I4">
-        <v>40.435000000000002</v>
+        <v>6.835</v>
       </c>
       <c r="J4">
-        <v>44.536999999999999</v>
+        <v>6.343</v>
       </c>
       <c r="K4">
-        <v>47.582000000000001</v>
+        <v>4.6619999999999999</v>
       </c>
       <c r="L4">
-        <v>50.6</v>
+        <v>3.718</v>
       </c>
       <c r="M4">
-        <v>52.959000000000003</v>
+        <v>3.9790000000000001</v>
       </c>
       <c r="N4">
-        <v>54.927999999999997</v>
+        <v>4.5250000000000004</v>
       </c>
       <c r="O4">
-        <v>57.113999999999997</v>
+        <v>4.78</v>
       </c>
       <c r="P4">
-        <v>59.698</v>
+        <v>2.6480000000000001</v>
       </c>
       <c r="Q4">
-        <v>62.552</v>
+        <v>2.1669999999999998</v>
       </c>
       <c r="R4">
-        <v>64.207999999999998</v>
+        <v>1.944</v>
       </c>
       <c r="S4">
-        <v>65.599999999999994</v>
+        <v>0.872</v>
       </c>
       <c r="T4">
-        <v>66.875</v>
+        <v>1.841</v>
       </c>
       <c r="U4">
-        <v>67.457999999999998</v>
+        <v>2.0379999999999998</v>
       </c>
       <c r="V4">
-        <v>68.7</v>
+        <v>2.0920000000000001</v>
       </c>
       <c r="W4">
-        <v>70.099999999999994</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="X4">
-        <v>71.566999999999993</v>
+        <v>1.3140000000000001</v>
       </c>
       <c r="Y4">
-        <v>72.95</v>
+        <v>2.0409999999999999</v>
       </c>
       <c r="Z4">
-        <v>73.908000000000001</v>
+        <v>2.7509999999999999</v>
       </c>
       <c r="AA4">
-        <v>75.417000000000002</v>
+        <v>2.2690000000000001</v>
       </c>
       <c r="AB4">
-        <v>77.492000000000004</v>
+        <v>2.3969999999999998</v>
       </c>
       <c r="AC4">
-        <v>79.25</v>
+        <v>1.9610000000000001</v>
       </c>
       <c r="AD4">
-        <v>81.150000000000006</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="AE4">
-        <v>82.742000000000004</v>
+        <v>1.726</v>
       </c>
       <c r="AF4">
-        <v>83.516999999999996</v>
+        <v>1.8440000000000001</v>
       </c>
       <c r="AG4">
-        <v>84.957999999999998</v>
+        <v>1.657</v>
       </c>
       <c r="AH4">
-        <v>86.525000000000006</v>
+        <v>3.6379999999999999</v>
       </c>
       <c r="AI4">
-        <v>87.957999999999998</v>
+        <v>1.042</v>
       </c>
       <c r="AJ4">
-        <v>91.158000000000001</v>
+        <v>2.198</v>
       </c>
       <c r="AK4">
-        <v>92.108000000000004</v>
+        <v>2.6560000000000001</v>
       </c>
       <c r="AL4">
-        <v>94.132999999999996</v>
+        <v>2.3540000000000001</v>
       </c>
       <c r="AM4">
-        <v>96.632999999999996</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="AN4">
-        <v>98.908000000000001</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="AO4">
-        <v>99.424999999999997</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="AP4">
-        <v>99.775000000000006</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AQ4">
-        <v>100</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="AR4">
-        <v>100.017</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="AS4">
-        <v>101.075</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="AT4">
-        <v>101.792</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="AU4">
-        <v>102.533</v>
+        <v>1.944</v>
       </c>
       <c r="AV4">
-        <v>102.875</v>
+        <v>8.5340000000000007</v>
       </c>
       <c r="AW4">
-        <v>104.875</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="AX4">
-        <v>113.825</v>
+        <v>2.8</v>
       </c>
       <c r="AY4">
-        <v>118.54900000000001</v>
+        <v>2.1</v>
       </c>
       <c r="AZ4">
-        <v>121.86799999999999</v>
+        <v>2.1</v>
       </c>
       <c r="BA4">
-        <v>124.42700000000001</v>
+        <v>2</v>
       </c>
       <c r="BB4">
-        <v>127.04</v>
+        <v>2</v>
       </c>
       <c r="BC4">
-        <v>129.58099999999999</v>
-      </c>
-      <c r="BD4">
-        <v>132.173</v>
-      </c>
-      <c r="BE4">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>37.753999999999998</v>
+      </c>
+      <c r="G5">
+        <v>42.435000000000002</v>
       </c>
       <c r="H5">
-        <v>11.339</v>
+        <v>46.179000000000002</v>
       </c>
       <c r="I5">
-        <v>11.718</v>
+        <v>48.987000000000002</v>
       </c>
       <c r="J5">
-        <v>10.146000000000001</v>
+        <v>51.795000000000002</v>
       </c>
       <c r="K5">
-        <v>6.835</v>
+        <v>53.563000000000002</v>
       </c>
       <c r="L5">
-        <v>6.343</v>
+        <v>55.954999999999998</v>
       </c>
       <c r="M5">
-        <v>4.6619999999999999</v>
+        <v>58.14</v>
       </c>
       <c r="N5">
-        <v>3.718</v>
+        <v>60.844000000000001</v>
       </c>
       <c r="O5">
-        <v>3.9790000000000001</v>
+        <v>63.756</v>
       </c>
       <c r="P5">
-        <v>4.5250000000000004</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="Q5">
-        <v>4.78</v>
+        <v>66.3</v>
       </c>
       <c r="R5">
-        <v>2.6480000000000001</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="S5">
-        <v>2.1669999999999998</v>
+        <v>67.8</v>
       </c>
       <c r="T5">
-        <v>1.944</v>
+        <v>69.5</v>
       </c>
       <c r="U5">
-        <v>0.872</v>
+        <v>70.7</v>
       </c>
       <c r="V5">
-        <v>1.841</v>
+        <v>72.3</v>
       </c>
       <c r="W5">
-        <v>2.0379999999999998</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="X5">
-        <v>2.0920000000000001</v>
+        <v>74.3</v>
       </c>
       <c r="Y5">
-        <v>1.9330000000000001</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="Z5">
-        <v>1.3140000000000001</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="AA5">
-        <v>2.0409999999999999</v>
+        <v>80</v>
       </c>
       <c r="AB5">
-        <v>2.7509999999999999</v>
+        <v>82.1</v>
       </c>
       <c r="AC5">
-        <v>2.2690000000000001</v>
+        <v>83.1</v>
       </c>
       <c r="AD5">
-        <v>2.3969999999999998</v>
+        <v>83.9</v>
       </c>
       <c r="AE5">
-        <v>1.9610000000000001</v>
+        <v>85.8</v>
       </c>
       <c r="AF5">
-        <v>0.93700000000000006</v>
+        <v>87.2</v>
       </c>
       <c r="AG5">
-        <v>1.726</v>
+        <v>89.4</v>
       </c>
       <c r="AH5">
-        <v>1.8440000000000001</v>
+        <v>91.6</v>
       </c>
       <c r="AI5">
-        <v>1.657</v>
+        <v>92.7</v>
       </c>
       <c r="AJ5">
-        <v>3.6379999999999999</v>
+        <v>95.3</v>
       </c>
       <c r="AK5">
-        <v>1.042</v>
+        <v>97.6</v>
       </c>
       <c r="AL5">
-        <v>2.198</v>
+        <v>99.3</v>
       </c>
       <c r="AM5">
-        <v>2.6560000000000001</v>
+        <v>99.8</v>
       </c>
       <c r="AN5">
-        <v>2.3540000000000001</v>
+        <v>99.8</v>
       </c>
       <c r="AO5">
-        <v>0.52200000000000002</v>
+        <v>100.1</v>
       </c>
       <c r="AP5">
-        <v>0.35199999999999998</v>
+        <v>100.4</v>
       </c>
       <c r="AQ5">
-        <v>0.22600000000000001</v>
+        <v>101.3</v>
       </c>
       <c r="AR5">
-        <v>1.7000000000000001E-2</v>
+        <v>102</v>
       </c>
       <c r="AS5">
-        <v>1.0580000000000001</v>
+        <v>102.9</v>
       </c>
       <c r="AT5">
-        <v>0.70899999999999996</v>
+        <v>103.4</v>
       </c>
       <c r="AU5">
-        <v>0.72899999999999998</v>
+        <v>107</v>
       </c>
       <c r="AV5">
-        <v>0.33300000000000002</v>
+        <v>117.3</v>
       </c>
       <c r="AW5">
-        <v>1.944</v>
+        <v>120.17400000000001</v>
       </c>
       <c r="AX5">
-        <v>8.5340000000000007</v>
+        <v>123.178</v>
       </c>
       <c r="AY5">
-        <v>4.1500000000000004</v>
+        <v>126.011</v>
       </c>
       <c r="AZ5">
-        <v>2.8</v>
+        <v>128.78399999999999</v>
       </c>
       <c r="BA5">
-        <v>2.1</v>
+        <v>131.488</v>
       </c>
       <c r="BB5">
-        <v>2.1</v>
+        <v>134.11799999999999</v>
       </c>
       <c r="BC5">
-        <v>2</v>
-      </c>
-      <c r="BD5">
-        <v>2</v>
-      </c>
-      <c r="BE5">
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
+      <c r="F6">
+        <v>10.670999999999999</v>
+      </c>
+      <c r="G6">
+        <v>12.397</v>
       </c>
       <c r="H6">
-        <v>37.753999999999998</v>
+        <v>8.8239999999999998</v>
       </c>
       <c r="I6">
-        <v>42.435000000000002</v>
+        <v>6.0810000000000004</v>
       </c>
       <c r="J6">
-        <v>46.179000000000002</v>
+        <v>5.7320000000000002</v>
       </c>
       <c r="K6">
-        <v>48.987000000000002</v>
+        <v>3.4140000000000001</v>
       </c>
       <c r="L6">
-        <v>51.795000000000002</v>
+        <v>4.4660000000000002</v>
       </c>
       <c r="M6">
-        <v>53.563000000000002</v>
+        <v>3.903</v>
       </c>
       <c r="N6">
-        <v>55.954999999999998</v>
+        <v>4.6509999999999998</v>
       </c>
       <c r="O6">
-        <v>58.14</v>
+        <v>4.7859999999999996</v>
       </c>
       <c r="P6">
-        <v>60.844000000000001</v>
+        <v>1.794</v>
       </c>
       <c r="Q6">
-        <v>63.756</v>
+        <v>2.157</v>
       </c>
       <c r="R6">
-        <v>64.900000000000006</v>
+        <v>1.2070000000000001</v>
       </c>
       <c r="S6">
-        <v>66.3</v>
+        <v>1.0429999999999999</v>
       </c>
       <c r="T6">
-        <v>67.099999999999994</v>
+        <v>2.5070000000000001</v>
       </c>
       <c r="U6">
-        <v>67.8</v>
+        <v>1.7270000000000001</v>
       </c>
       <c r="V6">
-        <v>69.5</v>
+        <v>2.2629999999999999</v>
       </c>
       <c r="W6">
-        <v>70.7</v>
+        <v>1.5209999999999999</v>
       </c>
       <c r="X6">
-        <v>72.3</v>
+        <v>1.226</v>
       </c>
       <c r="Y6">
-        <v>73.400000000000006</v>
+        <v>3.0960000000000001</v>
       </c>
       <c r="Z6">
-        <v>74.3</v>
+        <v>2.35</v>
       </c>
       <c r="AA6">
-        <v>76.599999999999994</v>
+        <v>2.0409999999999999</v>
       </c>
       <c r="AB6">
-        <v>78.400000000000006</v>
+        <v>2.625</v>
       </c>
       <c r="AC6">
-        <v>80</v>
+        <v>1.218</v>
       </c>
       <c r="AD6">
-        <v>82.1</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="AE6">
-        <v>83.1</v>
+        <v>2.2650000000000001</v>
       </c>
       <c r="AF6">
-        <v>83.9</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="AG6">
-        <v>85.8</v>
+        <v>2.5230000000000001</v>
       </c>
       <c r="AH6">
-        <v>87.2</v>
+        <v>2.4609999999999999</v>
       </c>
       <c r="AI6">
-        <v>89.4</v>
+        <v>1.2010000000000001</v>
       </c>
       <c r="AJ6">
-        <v>91.6</v>
+        <v>2.8050000000000002</v>
       </c>
       <c r="AK6">
-        <v>92.7</v>
+        <v>2.4129999999999998</v>
       </c>
       <c r="AL6">
-        <v>95.3</v>
+        <v>1.742</v>
       </c>
       <c r="AM6">
-        <v>97.6</v>
+        <v>0.504</v>
       </c>
       <c r="AN6">
-        <v>99.3</v>
+        <v>0</v>
       </c>
       <c r="AO6">
-        <v>99.8</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="AP6">
-        <v>99.8</v>
+        <v>0.3</v>
       </c>
       <c r="AQ6">
-        <v>100.1</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="AR6">
-        <v>100.4</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="AS6">
-        <v>101.3</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="AT6">
-        <v>102</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="AU6">
-        <v>102.9</v>
+        <v>3.4820000000000002</v>
       </c>
       <c r="AV6">
-        <v>103.4</v>
+        <v>9.6259999999999994</v>
       </c>
       <c r="AW6">
-        <v>107</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="AX6">
-        <v>117.3</v>
+        <v>2.5</v>
       </c>
       <c r="AY6">
-        <v>120.17400000000001</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AZ6">
-        <v>123.178</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="BA6">
-        <v>126.011</v>
+        <v>2.1</v>
       </c>
       <c r="BB6">
-        <v>128.78399999999999</v>
+        <v>2</v>
       </c>
       <c r="BC6">
-        <v>131.488</v>
-      </c>
-      <c r="BD6">
-        <v>134.11799999999999</v>
-      </c>
-      <c r="BE6">
         <v>2022</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
+      <c r="F7">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="G7">
+        <v>5.1239999999999997</v>
       </c>
       <c r="H7">
-        <v>10.670999999999999</v>
+        <v>5.1189999999999998</v>
       </c>
       <c r="I7">
-        <v>12.397</v>
+        <v>5.1159999999999997</v>
       </c>
       <c r="J7">
-        <v>8.8239999999999998</v>
+        <v>5.1120000000000001</v>
       </c>
       <c r="K7">
-        <v>6.0810000000000004</v>
+        <v>5.1109999999999998</v>
       </c>
       <c r="L7">
-        <v>5.7320000000000002</v>
+        <v>5.1159999999999997</v>
       </c>
       <c r="M7">
-        <v>3.4140000000000001</v>
+        <v>5.125</v>
       </c>
       <c r="N7">
-        <v>4.4660000000000002</v>
+        <v>5.1289999999999996</v>
       </c>
       <c r="O7">
-        <v>3.903</v>
+        <v>5.13</v>
       </c>
       <c r="P7">
-        <v>4.6509999999999998</v>
+        <v>5.1349999999999998</v>
       </c>
       <c r="Q7">
-        <v>4.7859999999999996</v>
+        <v>5.1459999999999999</v>
       </c>
       <c r="R7">
-        <v>1.794</v>
+        <v>5.1619999999999999</v>
       </c>
       <c r="S7">
-        <v>2.157</v>
+        <v>5.181</v>
       </c>
       <c r="T7">
-        <v>1.2070000000000001</v>
+        <v>5.1970000000000001</v>
       </c>
       <c r="U7">
-        <v>1.0429999999999999</v>
+        <v>5.2160000000000002</v>
       </c>
       <c r="V7">
-        <v>2.5070000000000001</v>
+        <v>5.2510000000000003</v>
       </c>
       <c r="W7">
-        <v>1.7270000000000001</v>
+        <v>5.2750000000000004</v>
       </c>
       <c r="X7">
-        <v>2.2629999999999999</v>
+        <v>5.2949999999999999</v>
       </c>
       <c r="Y7">
-        <v>1.5209999999999999</v>
+        <v>5.3140000000000001</v>
       </c>
       <c r="Z7">
-        <v>1.226</v>
+        <v>5.33</v>
       </c>
       <c r="AA7">
-        <v>3.0960000000000001</v>
+        <v>5.3490000000000002</v>
       </c>
       <c r="AB7">
-        <v>2.35</v>
+        <v>5.3680000000000003</v>
       </c>
       <c r="AC7">
-        <v>2.0409999999999999</v>
+        <v>5.3840000000000003</v>
       </c>
       <c r="AD7">
-        <v>2.625</v>
+        <v>5.3979999999999997</v>
       </c>
       <c r="AE7">
-        <v>1.218</v>
+        <v>5.4109999999999996</v>
       </c>
       <c r="AF7">
-        <v>0.96299999999999997</v>
+        <v>5.4269999999999996</v>
       </c>
       <c r="AG7">
-        <v>2.2650000000000001</v>
+        <v>5.4470000000000001</v>
       </c>
       <c r="AH7">
-        <v>1.6319999999999999</v>
+        <v>5.476</v>
       </c>
       <c r="AI7">
-        <v>2.5230000000000001</v>
+        <v>5.5110000000000001</v>
       </c>
       <c r="AJ7">
-        <v>2.4609999999999999</v>
+        <v>5.5350000000000001</v>
       </c>
       <c r="AK7">
-        <v>1.2010000000000001</v>
+        <v>5.5609999999999999</v>
       </c>
       <c r="AL7">
-        <v>2.8050000000000002</v>
+        <v>5.5810000000000004</v>
       </c>
       <c r="AM7">
-        <v>2.4129999999999998</v>
+        <v>5.6029999999999998</v>
       </c>
       <c r="AN7">
-        <v>1.742</v>
+        <v>5.6269999999999998</v>
       </c>
       <c r="AO7">
-        <v>0.504</v>
+        <v>5.66</v>
       </c>
       <c r="AP7">
-        <v>0</v>
+        <v>5.7069999999999999</v>
       </c>
       <c r="AQ7">
-        <v>0.30099999999999999</v>
+        <v>5.7489999999999997</v>
       </c>
       <c r="AR7">
-        <v>0.3</v>
+        <v>5.7809999999999997</v>
       </c>
       <c r="AS7">
-        <v>0.89600000000000002</v>
+        <v>5.806</v>
       </c>
       <c r="AT7">
-        <v>0.69099999999999995</v>
+        <v>5.8230000000000004</v>
       </c>
       <c r="AU7">
-        <v>0.88200000000000001</v>
+        <v>5.84</v>
       </c>
       <c r="AV7">
-        <v>0.48599999999999999</v>
+        <v>5.8730000000000002</v>
       </c>
       <c r="AW7">
-        <v>3.4820000000000002</v>
+        <v>5.8929999999999998</v>
       </c>
       <c r="AX7">
-        <v>9.6259999999999994</v>
+        <v>5.9119999999999999</v>
       </c>
       <c r="AY7">
-        <v>2.4500000000000002</v>
+        <v>5.9320000000000004</v>
       </c>
       <c r="AZ7">
-        <v>2.5</v>
+        <v>5.9530000000000003</v>
       </c>
       <c r="BA7">
-        <v>2.2999999999999998</v>
+        <v>5.9740000000000002</v>
       </c>
       <c r="BB7">
-        <v>2.2000000000000002</v>
+        <v>5.9960000000000004</v>
       </c>
       <c r="BC7">
-        <v>2.1</v>
-      </c>
-      <c r="BD7">
-        <v>2</v>
-      </c>
-      <c r="BE7">
         <v>2022</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8">
-        <v>5.1219999999999999</v>
-      </c>
-      <c r="I8">
-        <v>5.1239999999999997</v>
-      </c>
-      <c r="J8">
-        <v>5.1189999999999998</v>
-      </c>
-      <c r="K8">
-        <v>5.1159999999999997</v>
-      </c>
-      <c r="L8">
-        <v>5.1120000000000001</v>
-      </c>
-      <c r="M8">
-        <v>5.1109999999999998</v>
-      </c>
-      <c r="N8">
-        <v>5.1159999999999997</v>
-      </c>
-      <c r="O8">
-        <v>5.125</v>
-      </c>
-      <c r="P8">
-        <v>5.1289999999999996</v>
-      </c>
-      <c r="Q8">
-        <v>5.13</v>
-      </c>
-      <c r="R8">
-        <v>5.1349999999999998</v>
-      </c>
-      <c r="S8">
-        <v>5.1459999999999999</v>
-      </c>
-      <c r="T8">
-        <v>5.1619999999999999</v>
-      </c>
-      <c r="U8">
-        <v>5.181</v>
-      </c>
-      <c r="V8">
-        <v>5.1970000000000001</v>
-      </c>
-      <c r="W8">
-        <v>5.2160000000000002</v>
-      </c>
-      <c r="X8">
-        <v>5.2510000000000003</v>
-      </c>
-      <c r="Y8">
-        <v>5.2750000000000004</v>
-      </c>
-      <c r="Z8">
-        <v>5.2949999999999999</v>
-      </c>
-      <c r="AA8">
-        <v>5.3140000000000001</v>
-      </c>
-      <c r="AB8">
-        <v>5.33</v>
-      </c>
-      <c r="AC8">
-        <v>5.3490000000000002</v>
-      </c>
-      <c r="AD8">
-        <v>5.3680000000000003</v>
-      </c>
-      <c r="AE8">
-        <v>5.3840000000000003</v>
-      </c>
-      <c r="AF8">
-        <v>5.3979999999999997</v>
-      </c>
-      <c r="AG8">
-        <v>5.4109999999999996</v>
-      </c>
-      <c r="AH8">
-        <v>5.4269999999999996</v>
-      </c>
-      <c r="AI8">
-        <v>5.4470000000000001</v>
-      </c>
-      <c r="AJ8">
-        <v>5.476</v>
-      </c>
-      <c r="AK8">
-        <v>5.5110000000000001</v>
-      </c>
-      <c r="AL8">
-        <v>5.5350000000000001</v>
-      </c>
-      <c r="AM8">
-        <v>5.5609999999999999</v>
-      </c>
-      <c r="AN8">
-        <v>5.5810000000000004</v>
-      </c>
-      <c r="AO8">
-        <v>5.6029999999999998</v>
-      </c>
-      <c r="AP8">
-        <v>5.6269999999999998</v>
-      </c>
-      <c r="AQ8">
-        <v>5.66</v>
-      </c>
-      <c r="AR8">
-        <v>5.7069999999999999</v>
-      </c>
-      <c r="AS8">
-        <v>5.7489999999999997</v>
-      </c>
-      <c r="AT8">
-        <v>5.7809999999999997</v>
-      </c>
-      <c r="AU8">
-        <v>5.806</v>
-      </c>
-      <c r="AV8">
-        <v>5.8230000000000004</v>
-      </c>
-      <c r="AW8">
-        <v>5.84</v>
-      </c>
-      <c r="AX8">
-        <v>5.8730000000000002</v>
-      </c>
-      <c r="AY8">
-        <v>5.8929999999999998</v>
-      </c>
-      <c r="AZ8">
-        <v>5.9119999999999999</v>
-      </c>
-      <c r="BA8">
-        <v>5.9320000000000004</v>
-      </c>
-      <c r="BB8">
-        <v>5.9530000000000003</v>
-      </c>
-      <c r="BC8">
-        <v>5.9740000000000002</v>
-      </c>
-      <c r="BD8">
-        <v>5.9960000000000004</v>
-      </c>
-      <c r="BE8">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>32</v>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refreshed IMF WEO data with APR 25 forecasts
</commit_message>
<xml_diff>
--- a/Input data/WEO_Data_Denmark.xlsx
+++ b/Input data/WEO_Data_Denmark.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{612FA80C-C686-4BDC-B2D4-157A43494BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1A8657-FEFE-4BBB-A4B6-F71FF713F8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C864BDF0-D0DE-4681-BEAB-27177CA14C44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E4CAF8B-0065-4E9F-B52E-D099D83114AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="WEO_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="WEO_Data_Denmark" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -52,7 +52,7 @@
     <t>Billions</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 National accounts manual used: European System of Accounts (ESA) 2010 GDP valuation: Market prices Reporting in calendar year: Yes Start/end months of reporting year: January/December Base year: 2010 Chain-weighted: Yes, from 1980 Primary domestic currency: Danish krone Data last updated: 08/2024</t>
+    <t>Source: National Statistics Office Latest actual data: 2023 National accounts manual used: European System of Accounts (ESA) 2010 GDP valuation: Market prices Reporting in calendar year: Yes Start/end months of reporting year: January/December Base year: 2020 Chain-weighted: Yes, from 1980 Primary domestic currency: Danish krone Data last updated: 04/09/2025</t>
   </si>
   <si>
     <t>Inflation, average consumer prices</t>
@@ -61,7 +61,7 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 Harmonized prices: Yes Base year: 2015 Primary domestic currency: Danish krone Data last updated: 08/2024</t>
+    <t>Source: National Statistics Office Latest actual data: 2024 Harmonized prices: Yes Base year: 2015 Primary domestic currency: Danish krone Data last updated: 04/09/2025</t>
   </si>
   <si>
     <t>Percent change</t>
@@ -85,10 +85,10 @@
     <t>Millions</t>
   </si>
   <si>
-    <t>Source: National Statistics Office Latest actual data: 2022 Primary domestic currency: Danish krone Data last updated: 08/2024</t>
-  </si>
-  <si>
-    <t>International Monetary Fund, World Economic Outlook Database, October 2024</t>
+    <t>Source: National Statistics Office Latest actual data: 2024 Primary domestic currency: Danish krone Data last updated: 04/09/2025</t>
+  </si>
+  <si>
+    <t>International Monetary Fund, World Economic Outlook Database, April 2025</t>
   </si>
 </sst>
 </file>
@@ -949,14 +949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF687787-6652-4435-AA1E-9DD4120B4E02}">
-  <dimension ref="A1:BD9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF3D36B-5DBD-47F5-889A-D50B79EC0345}">
+  <dimension ref="A1:BE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1122,11 +1122,14 @@
       <c r="BC1">
         <v>2029</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1">
+        <v>2030</v>
+      </c>
+      <c r="BE1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1275,28 +1278,31 @@
         <v>2804.7429999999999</v>
       </c>
       <c r="AX2" s="1">
-        <v>2842.096</v>
+        <v>2960.8870000000002</v>
       </c>
       <c r="AY2" s="1">
-        <v>2964.279</v>
+        <v>3111.2629999999999</v>
       </c>
       <c r="AZ2" s="1">
-        <v>3066.6410000000001</v>
+        <v>3230.97</v>
       </c>
       <c r="BA2" s="1">
-        <v>3170.8620000000001</v>
+        <v>3349.7</v>
       </c>
       <c r="BB2" s="1">
-        <v>3280.8440000000001</v>
+        <v>3464.9749999999999</v>
       </c>
       <c r="BC2" s="1">
-        <v>3395.17</v>
-      </c>
-      <c r="BD2">
-        <v>2022</v>
+        <v>3586.9050000000002</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>3710.3530000000001</v>
+      </c>
+      <c r="BE2">
+        <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1445,28 +1451,31 @@
         <v>117.642</v>
       </c>
       <c r="AX3">
-        <v>119.759</v>
+        <v>119.133</v>
       </c>
       <c r="AY3">
-        <v>122.39400000000001</v>
+        <v>121.43899999999999</v>
       </c>
       <c r="AZ3">
-        <v>124.842</v>
+        <v>123.99</v>
       </c>
       <c r="BA3">
-        <v>127.339</v>
+        <v>126.46899999999999</v>
       </c>
       <c r="BB3">
-        <v>129.88499999999999</v>
+        <v>128.999</v>
       </c>
       <c r="BC3">
-        <v>132.483</v>
+        <v>131.57900000000001</v>
       </c>
       <c r="BD3">
-        <v>2022</v>
+        <v>134.21</v>
+      </c>
+      <c r="BE3">
+        <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1615,13 +1624,13 @@
         <v>3.3530000000000002</v>
       </c>
       <c r="AX4">
-        <v>1.8</v>
+        <v>1.268</v>
       </c>
       <c r="AY4">
-        <v>2.2000000000000002</v>
+        <v>1.9359999999999999</v>
       </c>
       <c r="AZ4">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="BA4">
         <v>2</v>
@@ -1633,10 +1642,13 @@
         <v>2</v>
       </c>
       <c r="BD4">
-        <v>2022</v>
+        <v>2</v>
+      </c>
+      <c r="BE4">
+        <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1782,31 +1794,34 @@
         <v>117.5</v>
       </c>
       <c r="AW5">
-        <v>118.1</v>
+        <v>118</v>
       </c>
       <c r="AX5">
-        <v>120.816</v>
+        <v>120.2</v>
       </c>
       <c r="AY5">
-        <v>123.233</v>
+        <v>122.744</v>
       </c>
       <c r="AZ5">
-        <v>125.697</v>
+        <v>125.322</v>
       </c>
       <c r="BA5">
-        <v>128.21100000000001</v>
+        <v>127.828</v>
       </c>
       <c r="BB5">
-        <v>130.77500000000001</v>
+        <v>130.38399999999999</v>
       </c>
       <c r="BC5">
-        <v>133.39099999999999</v>
+        <v>132.99199999999999</v>
       </c>
       <c r="BD5">
-        <v>2022</v>
+        <v>135.65199999999999</v>
+      </c>
+      <c r="BE5">
+        <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1952,16 +1967,16 @@
         <v>9.7110000000000003</v>
       </c>
       <c r="AW6">
-        <v>0.51100000000000001</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="AX6">
-        <v>2.2999999999999998</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="AY6">
-        <v>2</v>
+        <v>2.1160000000000001</v>
       </c>
       <c r="AZ6">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="BA6">
         <v>2</v>
@@ -1973,10 +1988,13 @@
         <v>2</v>
       </c>
       <c r="BD6">
-        <v>2022</v>
+        <v>2</v>
+      </c>
+      <c r="BE6">
+        <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2125,28 +2143,31 @@
         <v>5.9329999999999998</v>
       </c>
       <c r="AX7">
-        <v>5.952</v>
+        <v>5.9610000000000003</v>
       </c>
       <c r="AY7">
-        <v>5.992</v>
+        <v>6.0019999999999998</v>
       </c>
       <c r="AZ7">
-        <v>6.0369999999999999</v>
+        <v>6.0460000000000003</v>
       </c>
       <c r="BA7">
-        <v>6.0839999999999996</v>
+        <v>6.093</v>
       </c>
       <c r="BB7">
-        <v>6.14</v>
+        <v>6.15</v>
       </c>
       <c r="BC7">
-        <v>6.1740000000000004</v>
+        <v>6.1840000000000002</v>
       </c>
       <c r="BD7">
-        <v>2022</v>
+        <v>6.2270000000000003</v>
+      </c>
+      <c r="BE7">
+        <v>2024</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>

</xml_diff>